<commit_message>
update on Enterance Exam Module
kindly go through the changes and reviwe n then merge
</commit_message>
<xml_diff>
--- a/Book_Shop_System/Test Data/TestData.xlsx
+++ b/Book_Shop_System/Test Data/TestData.xlsx
@@ -1,48 +1,237 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20417"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KAIF KHAN\Desktop\Online_Book_Shop_System\Book_Shop\Book_Shop_System\Test Data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5987014A-47B5-46B3-A197-8FA884721B5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{443EE8BF-3E85-4AFE-A267-D0EB77750FED}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{797C52C8-CA55-4A50-A0A3-1C14D0DE00C4}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15660" windowHeight="6015" xr2:uid="{797C52C8-CA55-4A50-A0A3-1C14D0DE00C4}"/>
   </bookViews>
   <sheets>
-    <sheet name="Afshan Mansuri" sheetId="4" r:id="rId1"/>
+    <sheet name="AKmodule" sheetId="4" r:id="rId1"/>
     <sheet name="Kaif Khan" sheetId="5" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:E24"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="53">
+  <si>
+    <t>BookNmae</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entrance Exam </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Indian Economy </t>
+  </si>
+  <si>
+    <t>General Knowledge 2017</t>
+  </si>
+  <si>
+    <t>Kiran</t>
+  </si>
+  <si>
+    <t>Previous YearsSolved Papers &amp; 10 Practice Sets CMC (Vellore &amp; Ludhiana) Entrance Exam</t>
+  </si>
+  <si>
+    <t>IIM Indore IPM Full Length Test Series (Fully Solved)</t>
+  </si>
+  <si>
+    <t>Marketing Management</t>
+  </si>
+  <si>
+    <t>The Mega Yearbook 2016 - Current Affairs &amp; General Knowledge For Competitive Exams</t>
+  </si>
+  <si>
+    <t>Indian Polity (Civil Services Mains; Csat; Civil Services General)</t>
+  </si>
+  <si>
+    <t>Guide To RRB Non Technical Recruitment Exam</t>
+  </si>
+  <si>
+    <t>General Studies Paper 1</t>
+  </si>
+  <si>
+    <t>Mechanical Engineering</t>
+  </si>
+  <si>
+    <t>Literature and Fiction</t>
+  </si>
+  <si>
+    <t>Chetan Bhagat Collection</t>
+  </si>
+  <si>
+    <t>Ashwin Sanghi Boxset (Set Of 3 Books)</t>
+  </si>
+  <si>
+    <t>Tintin : Complete Adventures Of Tintin</t>
+  </si>
+  <si>
+    <t>Fifty Shades Trilogy (Set of 3 Books)</t>
+  </si>
+  <si>
+    <t>Code Red</t>
+  </si>
+  <si>
+    <t>Love . . . Not for Sale!</t>
+  </si>
+  <si>
+    <t>Ten Love Stories : An IndiBlogger Selection</t>
+  </si>
+  <si>
+    <t>Two Years Eight Months And Twentyeight Nights: A Novel</t>
+  </si>
+  <si>
+    <t>The Girl in the Spider's Web</t>
+  </si>
+  <si>
+    <t>You're Trending In My Dreams</t>
+  </si>
+  <si>
+    <t>Tell Me A Story</t>
+  </si>
+  <si>
+    <t>Go Set A Watchman</t>
+  </si>
+  <si>
+    <t>Academic and Professional</t>
+  </si>
+  <si>
+    <t>Getting A Coding Job For Dummies</t>
+  </si>
+  <si>
+    <t>What Next? A Complete Course &amp; Career Guide After Class 12 In Delhi NCR</t>
+  </si>
+  <si>
+    <t>Iit Foundation For Class-X Science</t>
+  </si>
+  <si>
+    <t>Research Analytics</t>
+  </si>
+  <si>
+    <t>Get a Grip on Grammar</t>
+  </si>
+  <si>
+    <t>Practical Business Analytics Using Sas-A Hands-On Guide</t>
+  </si>
+  <si>
+    <t>Engineering Physics 1st Edition</t>
+  </si>
+  <si>
+    <t>Chemistry For JEE Main And Advanced 2016 (Combo Set Of 3 Books)</t>
+  </si>
+  <si>
+    <t>Mechanics Of Materials</t>
+  </si>
+  <si>
+    <t>Python For Data Science For Dummies</t>
+  </si>
+  <si>
+    <t>Data Science And Big Data Analytics</t>
+  </si>
+  <si>
+    <t>Professional AngularJS</t>
+  </si>
+  <si>
+    <t>Biographies and Auto Biographies</t>
+  </si>
+  <si>
+    <t>Wings Of Fire: An Autobiography</t>
+  </si>
+  <si>
+    <t>The Z Factor : My Journey As The Wrong Man At The Right Time</t>
+  </si>
+  <si>
+    <t>Standing Guard: A Year In Opposition</t>
+  </si>
+  <si>
+    <t>The Turbulent Years: 1980 1996</t>
+  </si>
+  <si>
+    <t>Cracking The Code : My Journey To Bollywood</t>
+  </si>
+  <si>
+    <t>I Am Malala : The Girl Who Stood Up For Education And Was Shot By The Taliban</t>
+  </si>
+  <si>
+    <t>Being Salman</t>
+  </si>
+  <si>
+    <t>M.K. Gandhi An Autobiography</t>
+  </si>
+  <si>
+    <t>Steve Jobs</t>
+  </si>
+  <si>
+    <t>The Substance And The Shadow:An Autobiography Dilip Kumar</t>
+  </si>
+  <si>
+    <t>Shantaram</t>
+  </si>
+  <si>
+    <t>Courage And Conviction : An Autobiography</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Open sans"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFE43719"/>
+      <name val="Open sans"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Open sans"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFE43719"/>
+      <name val="Open sans"/>
     </font>
   </fonts>
   <fills count="2">
@@ -65,8 +254,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -381,13 +584,281 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F41BD8C2-5221-46C2-917A-1E2A249A1FB3}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B49"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="31.42578125" customWidth="1"/>
+    <col min="2" max="2" width="82.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="21" customHeight="1">
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="25.5">
+      <c r="B8" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="B9" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="B12" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="B13" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="B15" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="B16" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="B17" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="B18" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="B19" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="B20" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="B21" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="B22" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="B23" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="B24" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="B25" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="B27" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="B28" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="B29" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="B30" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="B31" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="B32" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="B33" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="B34" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="B35" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="B36" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="B37" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="B39" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="B40" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="B41" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="B42" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="B43" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="B44" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="B45" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="B46" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="B47" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="B48" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2">
+      <c r="B49" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -395,9 +866,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA053F04-BD89-4A6D-97BB-298F30F961A2}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
I have done new changes pleasw reviev and update
</commit_message>
<xml_diff>
--- a/Book_Shop_System/Test Data/TestData.xlsx
+++ b/Book_Shop_System/Test Data/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KAIF KHAN\Desktop\Online_Book_Shop_System\Book_Shop\Book_Shop_System\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5987014A-47B5-46B3-A197-8FA884721B5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E52A157C-7518-43EF-999E-7C7885BBF93B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{797C52C8-CA55-4A50-A0A3-1C14D0DE00C4}"/>
   </bookViews>
@@ -32,6 +32,17 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t>The Book Shop</t>
+  </si>
+  <si>
+    <t>Like a Love Song</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -393,12 +404,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA053F04-BD89-4A6D-97BB-298F30F961A2}">
-  <dimension ref="A1"/>
+  <dimension ref="A2:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
new update with respect to AAP and LAF module
kindly check and merge
</commit_message>
<xml_diff>
--- a/Book_Shop_System/Test Data/TestData.xlsx
+++ b/Book_Shop_System/Test Data/TestData.xlsx
@@ -3,16 +3,17 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20417"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{443EE8BF-3E85-4AFE-A267-D0EB77750FED}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{F521A870-52EF-480B-8C6A-036FFF502EDC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15660" windowHeight="6015" xr2:uid="{797C52C8-CA55-4A50-A0A3-1C14D0DE00C4}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15660" windowHeight="6015" activeTab="1" xr2:uid="{797C52C8-CA55-4A50-A0A3-1C14D0DE00C4}"/>
   </bookViews>
   <sheets>
     <sheet name="AKmodule" sheetId="4" r:id="rId1"/>
-    <sheet name="Kaif Khan" sheetId="5" r:id="rId2"/>
+    <sheet name="SortByoption" sheetId="6" r:id="rId2"/>
+    <sheet name="Kaif Khan" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:E24"/>
+  <oleSize ref="A1:P9"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="59">
   <si>
     <t>BookNmae</t>
   </si>
@@ -181,13 +182,31 @@
   </si>
   <si>
     <t>Courage And Conviction : An Autobiography</t>
+  </si>
+  <si>
+    <t>TC_ID</t>
+  </si>
+  <si>
+    <t>SortOption</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Low to High price</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Highest to Lowest price</t>
+  </si>
+  <si>
+    <t>Low to High discount</t>
+  </si>
+  <si>
+    <t>Highest to Lowest discount</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -233,6 +252,14 @@
       <color rgb="FFE43719"/>
       <name val="Open sans"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -254,7 +281,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -269,6 +296,12 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -586,8 +619,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F41BD8C2-5221-46C2-917A-1E2A249A1FB3}">
   <dimension ref="A1:B49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -863,6 +896,61 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17FDBA51-A95C-4384-B11F-C51DA36B1146}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2" ht="30">
+      <c r="A1" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="45">
+      <c r="A2" s="8">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="60">
+      <c r="A3" s="8">
+        <v>2</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="45">
+      <c r="A4" s="8">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="60">
+      <c r="A5" s="8">
+        <v>4</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA053F04-BD89-4A6D-97BB-298F30F961A2}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>